<commit_message>
BRS-701 minor data change (#67)
</commit_message>
<xml_diff>
--- a/migrations-data/20220825185430_data.xlsx
+++ b/migrations-data/20220825185430_data.xlsx
@@ -97,7 +97,7 @@
     <t xml:space="preserve">0509</t>
   </si>
   <si>
-    <t xml:space="preserve">Golden Ears Park - Golden Ears Group Camping</t>
+    <t xml:space="preserve">Golden Ears Park - Golden Ears Group Campground</t>
   </si>
   <si>
     <t xml:space="preserve">0510</t>
@@ -477,12 +477,12 @@
   <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I30" activeCellId="0" sqref="I30"/>
+      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="43.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="43.78"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>